<commit_message>
JAVA: [Eclipse] - Projekt "SnowRunner"
git-svn-id: file:///G/_svn_repo/programming/JAVA-Projects%20-%20Eclipse/SnowRunner@6048 8592820e-bdd2-cc16-cb4b-ca06df7e8abd
</commit_message>
<xml_diff>
--- a/DataStructures.xlsx
+++ b/DataStructures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__Data\Eclipse - Workspace\SnowRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9697BA87-2AE9-4B2A-BB9B-2CFDD618CE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E20D27-AF30-4E07-99BC-128FD2320BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6709E470-0187-4E89-80A3-7C58B1317277}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="72">
   <si>
     <t>TruckTire</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>GameDataTrailer</t>
+  </si>
+  <si>
+    <t>GameDataTruckAddon</t>
   </si>
 </sst>
 </file>
@@ -614,13 +617,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A8CAB6-91A1-4EE7-9823-CABC9BEE860A}">
-  <dimension ref="B1:AJ159"/>
+  <dimension ref="B1:AD159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="3" topLeftCell="G31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O55" sqref="O55"/>
+      <selection pane="bottomRight" activeCell="F125" sqref="F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1811,15 +1814,15 @@
     </row>
     <row r="41" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B41">
-        <f>SUMIF(I41:AD41,$E41,I$1:AD$1)</f>
+        <f t="shared" ref="B41:B59" si="23">SUMIF(I41:AD41,$E41,I$1:AD$1)</f>
         <v>8</v>
       </c>
       <c r="C41">
-        <f>SUMIF(I41:AD41,$E41,I$2:AD$2)</f>
+        <f t="shared" ref="C41:C59" si="24">SUMIF(I41:AD41,$E41,I$2:AD$2)</f>
         <v>255</v>
       </c>
       <c r="D41" s="4" t="str">
-        <f>TEXT(B41,"00")&amp;"_"&amp;TEXT(C41,"0000")</f>
+        <f t="shared" ref="D41:D59" si="25">TEXT(B41,"00")&amp;"_"&amp;TEXT(C41,"0000")</f>
         <v>08_0255</v>
       </c>
       <c r="E41" t="s">
@@ -1829,49 +1832,49 @@
         <v>66</v>
       </c>
       <c r="I41" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E41,I$5:I$21,0)),"",$E41)</f>
+        <f t="shared" ref="I41:I59" si="26">IF(ISERROR(MATCH($E41,I$5:I$21,0)),"",$E41)</f>
         <v>Price</v>
       </c>
       <c r="L41" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E41,L$5:L$21,0)),"",$E41)</f>
+        <f t="shared" ref="L41:L59" si="27">IF(ISERROR(MATCH($E41,L$5:L$21,0)),"",$E41)</f>
         <v>Price</v>
       </c>
       <c r="O41" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E41,O$5:O$21,0)),"",$E41)</f>
+        <f t="shared" ref="O41:O59" si="28">IF(ISERROR(MATCH($E41,O$5:O$21,0)),"",$E41)</f>
         <v>Price</v>
       </c>
       <c r="R41" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E41,R$5:R$21,0)),"",$E41)</f>
+        <f t="shared" ref="R41:R59" si="29">IF(ISERROR(MATCH($E41,R$5:R$21,0)),"",$E41)</f>
         <v>Price</v>
       </c>
       <c r="U41" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E41,U$5:U$21,0)),"",$E41)</f>
+        <f t="shared" ref="U41:U59" si="30">IF(ISERROR(MATCH($E41,U$5:U$21,0)),"",$E41)</f>
         <v>Price</v>
       </c>
       <c r="X41" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E41,X$5:X$21,0)),"",$E41)</f>
+        <f t="shared" ref="X41:X59" si="31">IF(ISERROR(MATCH($E41,X$5:X$21,0)),"",$E41)</f>
         <v>Price</v>
       </c>
       <c r="AA41" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E41,AA$5:AA$21,0)),"",$E41)</f>
+        <f t="shared" ref="AA41:AA59" si="32">IF(ISERROR(MATCH($E41,AA$5:AA$21,0)),"",$E41)</f>
         <v>Price</v>
       </c>
       <c r="AD41" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E41,AD$5:AD$21,0)),"",$E41)</f>
+        <f t="shared" ref="AD41:AD59" si="33">IF(ISERROR(MATCH($E41,AD$5:AD$21,0)),"",$E41)</f>
         <v>Price</v>
       </c>
     </row>
     <row r="42" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B42">
-        <f>SUMIF(I42:AD42,$E42,I$1:AD$1)</f>
+        <f t="shared" si="23"/>
         <v>8</v>
       </c>
       <c r="C42">
-        <f>SUMIF(I42:AD42,$E42,I$2:AD$2)</f>
+        <f t="shared" si="24"/>
         <v>255</v>
       </c>
       <c r="D42" s="4" t="str">
-        <f>TEXT(B42,"00")&amp;"_"&amp;TEXT(C42,"0000")</f>
+        <f t="shared" si="25"/>
         <v>08_0255</v>
       </c>
       <c r="E42" t="s">
@@ -1881,49 +1884,49 @@
         <v>66</v>
       </c>
       <c r="I42" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E42,I$5:I$21,0)),"",$E42)</f>
+        <f t="shared" si="26"/>
         <v>UnlockByExploration</v>
       </c>
       <c r="L42" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E42,L$5:L$21,0)),"",$E42)</f>
+        <f t="shared" si="27"/>
         <v>UnlockByExploration</v>
       </c>
       <c r="O42" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E42,O$5:O$21,0)),"",$E42)</f>
+        <f t="shared" si="28"/>
         <v>UnlockByExploration</v>
       </c>
       <c r="R42" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E42,R$5:R$21,0)),"",$E42)</f>
+        <f t="shared" si="29"/>
         <v>UnlockByExploration</v>
       </c>
       <c r="U42" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E42,U$5:U$21,0)),"",$E42)</f>
+        <f t="shared" si="30"/>
         <v>UnlockByExploration</v>
       </c>
       <c r="X42" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E42,X$5:X$21,0)),"",$E42)</f>
+        <f t="shared" si="31"/>
         <v>UnlockByExploration</v>
       </c>
       <c r="AA42" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E42,AA$5:AA$21,0)),"",$E42)</f>
+        <f t="shared" si="32"/>
         <v>UnlockByExploration</v>
       </c>
       <c r="AD42" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E42,AD$5:AD$21,0)),"",$E42)</f>
+        <f t="shared" si="33"/>
         <v>UnlockByExploration</v>
       </c>
     </row>
     <row r="43" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B43">
-        <f>SUMIF(I43:AD43,$E43,I$1:AD$1)</f>
+        <f t="shared" si="23"/>
         <v>8</v>
       </c>
       <c r="C43">
-        <f>SUMIF(I43:AD43,$E43,I$2:AD$2)</f>
+        <f t="shared" si="24"/>
         <v>255</v>
       </c>
       <c r="D43" s="4" t="str">
-        <f>TEXT(B43,"00")&amp;"_"&amp;TEXT(C43,"0000")</f>
+        <f t="shared" si="25"/>
         <v>08_0255</v>
       </c>
       <c r="E43" t="s">
@@ -1933,49 +1936,49 @@
         <v>66</v>
       </c>
       <c r="I43" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E43,I$5:I$21,0)),"",$E43)</f>
+        <f t="shared" si="26"/>
         <v>UnlockByRank</v>
       </c>
       <c r="L43" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E43,L$5:L$21,0)),"",$E43)</f>
+        <f t="shared" si="27"/>
         <v>UnlockByRank</v>
       </c>
       <c r="O43" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E43,O$5:O$21,0)),"",$E43)</f>
+        <f t="shared" si="28"/>
         <v>UnlockByRank</v>
       </c>
       <c r="R43" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E43,R$5:R$21,0)),"",$E43)</f>
+        <f t="shared" si="29"/>
         <v>UnlockByRank</v>
       </c>
       <c r="U43" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E43,U$5:U$21,0)),"",$E43)</f>
+        <f t="shared" si="30"/>
         <v>UnlockByRank</v>
       </c>
       <c r="X43" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E43,X$5:X$21,0)),"",$E43)</f>
+        <f t="shared" si="31"/>
         <v>UnlockByRank</v>
       </c>
       <c r="AA43" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E43,AA$5:AA$21,0)),"",$E43)</f>
+        <f t="shared" si="32"/>
         <v>UnlockByRank</v>
       </c>
       <c r="AD43" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E43,AD$5:AD$21,0)),"",$E43)</f>
+        <f t="shared" si="33"/>
         <v>UnlockByRank</v>
       </c>
     </row>
     <row r="44" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B44">
-        <f>SUMIF(I44:AD44,$E44,I$1:AD$1)</f>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="C44">
-        <f>SUMIF(I44:AD44,$E44,I$2:AD$2)</f>
+        <f t="shared" si="24"/>
         <v>7</v>
       </c>
       <c r="D44" s="4" t="str">
-        <f>TEXT(B44,"00")&amp;"_"&amp;TEXT(C44,"0000")</f>
+        <f t="shared" si="25"/>
         <v>03_0007</v>
       </c>
       <c r="E44" t="s">
@@ -1985,588 +1988,621 @@
         <v>67</v>
       </c>
       <c r="I44" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E44,I$5:I$21,0)),"",$E44)</f>
+        <f t="shared" si="26"/>
         <v>ExcludedCargoTypes</v>
       </c>
       <c r="L44" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E44,L$5:L$21,0)),"",$E44)</f>
+        <f t="shared" si="27"/>
         <v>ExcludedCargoTypes</v>
       </c>
       <c r="O44" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E44,O$5:O$21,0)),"",$E44)</f>
+        <f t="shared" si="28"/>
         <v>ExcludedCargoTypes</v>
       </c>
       <c r="R44" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E44,R$5:R$21,0)),"",$E44)</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="U44" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E44,U$5:U$21,0)),"",$E44)</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="X44" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E44,X$5:X$21,0)),"",$E44)</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="AA44" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E44,AA$5:AA$21,0)),"",$E44)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="AD44" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E44,AD$5:AD$21,0)),"",$E44)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
     </row>
     <row r="45" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B45">
-        <f>SUMIF(I45:AD45,$E45,I$1:AD$1)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="C45">
-        <f>SUMIF(I45:AD45,$E45,I$2:AD$2)</f>
+        <f t="shared" si="24"/>
         <v>4</v>
       </c>
       <c r="D45" s="4" t="str">
-        <f>TEXT(B45,"00")&amp;"_"&amp;TEXT(C45,"0000")</f>
+        <f t="shared" si="25"/>
         <v>01_0004</v>
       </c>
       <c r="E45" t="s">
         <v>27</v>
       </c>
+      <c r="F45" t="s">
+        <v>71</v>
+      </c>
       <c r="I45" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E45,I$5:I$21,0)),"",$E45)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="L45" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E45,L$5:L$21,0)),"",$E45)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="O45" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E45,O$5:O$21,0)),"",$E45)</f>
+        <f t="shared" si="28"/>
         <v>Category</v>
       </c>
       <c r="R45" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E45,R$5:R$21,0)),"",$E45)</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="U45" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E45,U$5:U$21,0)),"",$E45)</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="X45" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E45,X$5:X$21,0)),"",$E45)</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="AA45" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E45,AA$5:AA$21,0)),"",$E45)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="AD45" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E45,AD$5:AD$21,0)),"",$E45)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B46">
-        <f>SUMIF(I46:AD46,$E46,I$1:AD$1)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="C46">
-        <f>SUMIF(I46:AD46,$E46,I$2:AD$2)</f>
+        <f t="shared" si="24"/>
         <v>4</v>
       </c>
       <c r="D46" s="4" t="str">
-        <f>TEXT(B46,"00")&amp;"_"&amp;TEXT(C46,"0000")</f>
+        <f t="shared" si="25"/>
         <v>01_0004</v>
       </c>
       <c r="E46" t="s">
         <v>28</v>
       </c>
+      <c r="F46" t="s">
+        <v>71</v>
+      </c>
       <c r="I46" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E46,I$5:I$21,0)),"",$E46)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="L46" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E46,L$5:L$21,0)),"",$E46)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="O46" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E46,O$5:O$21,0)),"",$E46)</f>
+        <f t="shared" si="28"/>
         <v>GaragePoints</v>
       </c>
       <c r="R46" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E46,R$5:R$21,0)),"",$E46)</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="U46" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E46,U$5:U$21,0)),"",$E46)</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="X46" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E46,X$5:X$21,0)),"",$E46)</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="AA46" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E46,AA$5:AA$21,0)),"",$E46)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="AD46" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E46,AD$5:AD$21,0)),"",$E46)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
     </row>
     <row r="47" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B47">
-        <f>SUMIF(I47:AD47,$E47,I$1:AD$1)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="C47">
-        <f>SUMIF(I47:AD47,$E47,I$2:AD$2)</f>
+        <f t="shared" si="24"/>
         <v>4</v>
       </c>
       <c r="D47" s="4" t="str">
-        <f>TEXT(B47,"00")&amp;"_"&amp;TEXT(C47,"0000")</f>
+        <f t="shared" si="25"/>
         <v>01_0004</v>
       </c>
       <c r="E47" t="s">
         <v>29</v>
       </c>
+      <c r="F47" t="s">
+        <v>71</v>
+      </c>
       <c r="I47" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E47,I$5:I$21,0)),"",$E47)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="L47" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E47,L$5:L$21,0)),"",$E47)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="O47" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E47,O$5:O$21,0)),"",$E47)</f>
+        <f t="shared" si="28"/>
         <v>IsCustomizable</v>
       </c>
       <c r="R47" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E47,R$5:R$21,0)),"",$E47)</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="U47" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E47,U$5:U$21,0)),"",$E47)</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="X47" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E47,X$5:X$21,0)),"",$E47)</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="AA47" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E47,AA$5:AA$21,0)),"",$E47)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="AD47" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E47,AD$5:AD$21,0)),"",$E47)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
     </row>
     <row r="48" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B48">
-        <f>SUMIF(I48:AD48,$E48,I$1:AD$1)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="C48">
-        <f>SUMIF(I48:AD48,$E48,I$2:AD$2)</f>
+        <f t="shared" si="24"/>
         <v>4</v>
       </c>
       <c r="D48" s="4" t="str">
-        <f>TEXT(B48,"00")&amp;"_"&amp;TEXT(C48,"0000")</f>
+        <f t="shared" si="25"/>
         <v>01_0004</v>
       </c>
       <c r="E48" t="s">
         <v>30</v>
       </c>
+      <c r="F48" t="s">
+        <v>71</v>
+      </c>
       <c r="I48" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E48,I$5:I$21,0)),"",$E48)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="L48" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E48,L$5:L$21,0)),"",$E48)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="O48" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E48,O$5:O$21,0)),"",$E48)</f>
+        <f t="shared" si="28"/>
         <v>LoadPoints</v>
       </c>
       <c r="R48" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E48,R$5:R$21,0)),"",$E48)</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="U48" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E48,U$5:U$21,0)),"",$E48)</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="X48" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E48,X$5:X$21,0)),"",$E48)</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="AA48" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E48,AA$5:AA$21,0)),"",$E48)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="AD48" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E48,AD$5:AD$21,0)),"",$E48)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
     </row>
     <row r="49" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B49">
-        <f>SUMIF(I49:AD49,$E49,I$1:AD$1)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="C49">
-        <f>SUMIF(I49:AD49,$E49,I$2:AD$2)</f>
+        <f t="shared" si="24"/>
         <v>4</v>
       </c>
       <c r="D49" s="4" t="str">
-        <f>TEXT(B49,"00")&amp;"_"&amp;TEXT(C49,"0000")</f>
+        <f t="shared" si="25"/>
         <v>01_0004</v>
       </c>
       <c r="E49" t="s">
         <v>31</v>
       </c>
+      <c r="F49" t="s">
+        <v>71</v>
+      </c>
       <c r="I49" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E49,I$5:I$21,0)),"",$E49)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="L49" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E49,L$5:L$21,0)),"",$E49)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="O49" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E49,O$5:O$21,0)),"",$E49)</f>
+        <f t="shared" si="28"/>
         <v>ManualLoads</v>
       </c>
       <c r="R49" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E49,R$5:R$21,0)),"",$E49)</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="U49" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E49,U$5:U$21,0)),"",$E49)</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="X49" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E49,X$5:X$21,0)),"",$E49)</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="AA49" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E49,AA$5:AA$21,0)),"",$E49)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="AD49" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E49,AD$5:AD$21,0)),"",$E49)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
     </row>
     <row r="50" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B50">
-        <f>SUMIF(I50:AD50,$E50,I$1:AD$1)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="C50">
-        <f>SUMIF(I50:AD50,$E50,I$2:AD$2)</f>
+        <f t="shared" si="24"/>
         <v>4</v>
       </c>
       <c r="D50" s="4" t="str">
-        <f>TEXT(B50,"00")&amp;"_"&amp;TEXT(C50,"0000")</f>
+        <f t="shared" si="25"/>
         <v>01_0004</v>
       </c>
       <c r="E50" t="s">
         <v>32</v>
       </c>
+      <c r="F50" t="s">
+        <v>71</v>
+      </c>
       <c r="I50" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E50,I$5:I$21,0)),"",$E50)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="L50" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E50,L$5:L$21,0)),"",$E50)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="O50" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E50,O$5:O$21,0)),"",$E50)</f>
+        <f t="shared" si="28"/>
         <v>OriginalAddon</v>
       </c>
       <c r="R50" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E50,R$5:R$21,0)),"",$E50)</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="U50" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E50,U$5:U$21,0)),"",$E50)</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="X50" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E50,X$5:X$21,0)),"",$E50)</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="AA50" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E50,AA$5:AA$21,0)),"",$E50)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="AD50" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E50,AD$5:AD$21,0)),"",$E50)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
     </row>
     <row r="51" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B51">
-        <f>SUMIF(I51:AD51,$E51,I$1:AD$1)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="C51">
-        <f>SUMIF(I51:AD51,$E51,I$2:AD$2)</f>
+        <f t="shared" si="24"/>
         <v>4</v>
       </c>
       <c r="D51" s="4" t="str">
-        <f>TEXT(B51,"00")&amp;"_"&amp;TEXT(C51,"0000")</f>
+        <f t="shared" si="25"/>
         <v>01_0004</v>
       </c>
       <c r="E51" t="s">
         <v>33</v>
       </c>
+      <c r="F51" t="s">
+        <v>71</v>
+      </c>
       <c r="I51" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E51,I$5:I$21,0)),"",$E51)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="L51" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E51,L$5:L$21,0)),"",$E51)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="O51" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E51,O$5:O$21,0)),"",$E51)</f>
+        <f t="shared" si="28"/>
         <v>SaddleType</v>
       </c>
       <c r="R51" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E51,R$5:R$21,0)),"",$E51)</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="U51" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E51,U$5:U$21,0)),"",$E51)</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="X51" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E51,X$5:X$21,0)),"",$E51)</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="AA51" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E51,AA$5:AA$21,0)),"",$E51)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="AD51" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E51,AD$5:AD$21,0)),"",$E51)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B52">
-        <f>SUMIF(I52:AD52,$E52,I$1:AD$1)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="C52">
-        <f>SUMIF(I52:AD52,$E52,I$2:AD$2)</f>
+        <f t="shared" si="24"/>
         <v>4</v>
       </c>
       <c r="D52" s="4" t="str">
-        <f>TEXT(B52,"00")&amp;"_"&amp;TEXT(C52,"0000")</f>
+        <f t="shared" si="25"/>
         <v>01_0004</v>
       </c>
       <c r="E52" t="s">
         <v>34</v>
       </c>
+      <c r="F52" t="s">
+        <v>71</v>
+      </c>
       <c r="I52" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E52,I$5:I$21,0)),"",$E52)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="L52" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E52,L$5:L$21,0)),"",$E52)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="O52" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E52,O$5:O$21,0)),"",$E52)</f>
+        <f t="shared" si="28"/>
         <v>ShowPackingStoppers</v>
       </c>
       <c r="R52" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E52,R$5:R$21,0)),"",$E52)</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="U52" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E52,U$5:U$21,0)),"",$E52)</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="X52" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E52,X$5:X$21,0)),"",$E52)</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="AA52" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E52,AA$5:AA$21,0)),"",$E52)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="AD52" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E52,AD$5:AD$21,0)),"",$E52)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
     </row>
     <row r="53" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B53">
-        <f>SUMIF(I53:AD53,$E53,I$1:AD$1)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="C53">
-        <f>SUMIF(I53:AD53,$E53,I$2:AD$2)</f>
+        <f t="shared" si="24"/>
         <v>4</v>
       </c>
       <c r="D53" s="4" t="str">
-        <f>TEXT(B53,"00")&amp;"_"&amp;TEXT(C53,"0000")</f>
+        <f t="shared" si="25"/>
         <v>01_0004</v>
       </c>
       <c r="E53" t="s">
         <v>36</v>
       </c>
+      <c r="F53" t="s">
+        <v>71</v>
+      </c>
       <c r="I53" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E53,I$5:I$21,0)),"",$E53)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="L53" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E53,L$5:L$21,0)),"",$E53)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="O53" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E53,O$5:O$21,0)),"",$E53)</f>
+        <f t="shared" si="28"/>
         <v>TrialsToUnlock</v>
       </c>
       <c r="R53" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E53,R$5:R$21,0)),"",$E53)</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="U53" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E53,U$5:U$21,0)),"",$E53)</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="X53" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E53,X$5:X$21,0)),"",$E53)</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="AA53" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E53,AA$5:AA$21,0)),"",$E53)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="AD53" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E53,AD$5:AD$21,0)),"",$E53)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
     </row>
     <row r="54" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B54">
-        <f>SUMIF(I54:AD54,$E54,I$1:AD$1)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="C54">
-        <f>SUMIF(I54:AD54,$E54,I$2:AD$2)</f>
+        <f t="shared" si="24"/>
         <v>4</v>
       </c>
       <c r="D54" s="4" t="str">
-        <f>TEXT(B54,"00")&amp;"_"&amp;TEXT(C54,"0000")</f>
+        <f t="shared" si="25"/>
         <v>01_0004</v>
       </c>
       <c r="E54" t="s">
         <v>37</v>
       </c>
+      <c r="F54" t="s">
+        <v>71</v>
+      </c>
       <c r="I54" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E54,I$5:I$21,0)),"",$E54)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="L54" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E54,L$5:L$21,0)),"",$E54)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="O54" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E54,O$5:O$21,0)),"",$E54)</f>
+        <f t="shared" si="28"/>
         <v>UnpackOnTrailerDetach</v>
       </c>
       <c r="R54" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E54,R$5:R$21,0)),"",$E54)</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="U54" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E54,U$5:U$21,0)),"",$E54)</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="X54" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E54,X$5:X$21,0)),"",$E54)</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="AA54" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E54,AA$5:AA$21,0)),"",$E54)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="AD54" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E54,AD$5:AD$21,0)),"",$E54)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
     </row>
     <row r="55" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B55">
-        <f>SUMIF(I55:AD55,$E55,I$1:AD$1)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="C55">
-        <f>SUMIF(I55:AD55,$E55,I$2:AD$2)</f>
+        <f t="shared" si="24"/>
         <v>4</v>
       </c>
       <c r="D55" s="4" t="str">
-        <f>TEXT(B55,"00")&amp;"_"&amp;TEXT(C55,"0000")</f>
+        <f t="shared" si="25"/>
         <v>01_0004</v>
       </c>
       <c r="E55" t="s">
         <v>38</v>
       </c>
+      <c r="F55" t="s">
+        <v>71</v>
+      </c>
       <c r="I55" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E55,I$5:I$21,0)),"",$E55)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="L55" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E55,L$5:L$21,0)),"",$E55)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="O55" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E55,O$5:O$21,0)),"",$E55)</f>
+        <f t="shared" si="28"/>
         <v>WheelToPack</v>
       </c>
       <c r="R55" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E55,R$5:R$21,0)),"",$E55)</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="U55" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E55,U$5:U$21,0)),"",$E55)</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="X55" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E55,X$5:X$21,0)),"",$E55)</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="AA55" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E55,AA$5:AA$21,0)),"",$E55)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="AD55" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E55,AD$5:AD$21,0)),"",$E55)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
     </row>
     <row r="56" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B56">
-        <f>SUMIF(I56:AD56,$E56,I$1:AD$1)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="C56">
-        <f>SUMIF(I56:AD56,$E56,I$2:AD$2)</f>
+        <f t="shared" si="24"/>
         <v>2</v>
       </c>
       <c r="D56" s="4" t="str">
-        <f>TEXT(B56,"00")&amp;"_"&amp;TEXT(C56,"0000")</f>
+        <f t="shared" si="25"/>
         <v>01_0002</v>
       </c>
       <c r="E56" t="s">
@@ -2576,49 +2612,49 @@
         <v>70</v>
       </c>
       <c r="I56" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E56,I$5:I$21,0)),"",$E56)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="L56" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E56,L$5:L$21,0)),"",$E56)</f>
+        <f t="shared" si="27"/>
         <v>IsQuest</v>
       </c>
       <c r="O56" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E56,O$5:O$21,0)),"",$E56)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="R56" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E56,R$5:R$21,0)),"",$E56)</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="U56" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E56,U$5:U$21,0)),"",$E56)</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="X56" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E56,X$5:X$21,0)),"",$E56)</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="AA56" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E56,AA$5:AA$21,0)),"",$E56)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="AD56" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E56,AD$5:AD$21,0)),"",$E56)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
     </row>
     <row r="57" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B57">
-        <f>SUMIF(I57:AD57,$E57,I$1:AD$1)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="C57">
-        <f>SUMIF(I57:AD57,$E57,I$2:AD$2)</f>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D57" s="4" t="str">
-        <f>TEXT(B57,"00")&amp;"_"&amp;TEXT(C57,"0000")</f>
+        <f t="shared" si="25"/>
         <v>01_0001</v>
       </c>
       <c r="E57" t="s">
@@ -2628,49 +2664,49 @@
         <v>69</v>
       </c>
       <c r="I57" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E57,I$5:I$21,0)),"",$E57)</f>
+        <f t="shared" si="26"/>
         <v>Country</v>
       </c>
       <c r="L57" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E57,L$5:L$21,0)),"",$E57)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="O57" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E57,O$5:O$21,0)),"",$E57)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="R57" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E57,R$5:R$21,0)),"",$E57)</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="U57" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E57,U$5:U$21,0)),"",$E57)</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="X57" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E57,X$5:X$21,0)),"",$E57)</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="AA57" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E57,AA$5:AA$21,0)),"",$E57)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="AD57" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E57,AD$5:AD$21,0)),"",$E57)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
     </row>
     <row r="58" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B58">
-        <f>SUMIF(I58:AD58,$E58,I$1:AD$1)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="C58">
-        <f>SUMIF(I58:AD58,$E58,I$2:AD$2)</f>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D58" s="4" t="str">
-        <f>TEXT(B58,"00")&amp;"_"&amp;TEXT(C58,"0000")</f>
+        <f t="shared" si="25"/>
         <v>01_0001</v>
       </c>
       <c r="E58" t="s">
@@ -2680,49 +2716,49 @@
         <v>69</v>
       </c>
       <c r="I58" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E58,I$5:I$21,0)),"",$E58)</f>
+        <f t="shared" si="26"/>
         <v>ExcludeAddons</v>
       </c>
       <c r="L58" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E58,L$5:L$21,0)),"",$E58)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="O58" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E58,O$5:O$21,0)),"",$E58)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="R58" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E58,R$5:R$21,0)),"",$E58)</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="U58" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E58,U$5:U$21,0)),"",$E58)</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="X58" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E58,X$5:X$21,0)),"",$E58)</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="AA58" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E58,AA$5:AA$21,0)),"",$E58)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="AD58" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E58,AD$5:AD$21,0)),"",$E58)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
     </row>
     <row r="59" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B59">
-        <f>SUMIF(I59:AD59,$E59,I$1:AD$1)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="C59">
-        <f>SUMIF(I59:AD59,$E59,I$2:AD$2)</f>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D59" s="4" t="str">
-        <f>TEXT(B59,"00")&amp;"_"&amp;TEXT(C59,"0000")</f>
+        <f t="shared" si="25"/>
         <v>01_0001</v>
       </c>
       <c r="E59" t="s">
@@ -2732,35 +2768,35 @@
         <v>69</v>
       </c>
       <c r="I59" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E59,I$5:I$21,0)),"",$E59)</f>
+        <f t="shared" si="26"/>
         <v>Recallable</v>
       </c>
       <c r="L59" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E59,L$5:L$21,0)),"",$E59)</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="O59" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E59,O$5:O$21,0)),"",$E59)</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="R59" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E59,R$5:R$21,0)),"",$E59)</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="U59" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E59,U$5:U$21,0)),"",$E59)</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="X59" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E59,X$5:X$21,0)),"",$E59)</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="AA59" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E59,AA$5:AA$21,0)),"",$E59)</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="AD59" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E59,AD$5:AD$21,0)),"",$E59)</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
     </row>
@@ -3459,11 +3495,11 @@
     </row>
     <row r="90" spans="8:30" x14ac:dyDescent="0.25">
       <c r="I90" s="1" t="str">
-        <f t="shared" ref="I90" si="23">IF(H62="+",I62,IF(H62="-","",IF(I62="","","??????")))</f>
+        <f t="shared" ref="I90" si="34">IF(H62="+",I62,IF(H62="-","",IF(I62="","","??????")))</f>
         <v>AddonSlots</v>
       </c>
       <c r="L90" s="1" t="str">
-        <f t="shared" ref="L90" si="24">IF(K62="+",L62,IF(K62="-","",IF(L62="","","??????")))</f>
+        <f t="shared" ref="L90" si="35">IF(K62="+",L62,IF(K62="-","",IF(L62="","","??????")))</f>
         <v>AddonSlots</v>
       </c>
       <c r="O90" s="1" t="str">
@@ -3471,33 +3507,33 @@
         <v>AddonSlots</v>
       </c>
       <c r="R90" s="1" t="str">
-        <f t="shared" ref="R90" si="25">IF(Q62="+",R62,IF(Q62="-","",IF(R62="","","??????")))</f>
+        <f t="shared" ref="R90" si="36">IF(Q62="+",R62,IF(Q62="-","",IF(R62="","","??????")))</f>
         <v>UiDesc</v>
       </c>
       <c r="U90" s="1" t="str">
-        <f t="shared" ref="U90" si="26">IF(T62="+",U62,IF(T62="-","",IF(U62="","","??????")))</f>
+        <f t="shared" ref="U90" si="37">IF(T62="+",U62,IF(T62="-","",IF(U62="","","??????")))</f>
         <v/>
       </c>
       <c r="X90" s="1" t="str">
-        <f t="shared" ref="X90" si="27">IF(W62="+",X62,IF(W62="-","",IF(X62="","","??????")))</f>
+        <f t="shared" ref="X90" si="38">IF(W62="+",X62,IF(W62="-","",IF(X62="","","??????")))</f>
         <v>UiDesc</v>
       </c>
       <c r="AA90" s="1" t="str">
-        <f t="shared" ref="AA90" si="28">IF(Z62="+",AA62,IF(Z62="-","",IF(AA62="","","??????")))</f>
+        <f t="shared" ref="AA90" si="39">IF(Z62="+",AA62,IF(Z62="-","",IF(AA62="","","??????")))</f>
         <v>UiDesc</v>
       </c>
       <c r="AD90" s="1" t="str">
-        <f t="shared" ref="AD90:AD91" si="29">IF(AC62="+",AD62,IF(AC62="-","",IF(AD62="","","??????")))</f>
+        <f t="shared" ref="AD90:AD91" si="40">IF(AC62="+",AD62,IF(AC62="-","",IF(AD62="","","??????")))</f>
         <v>UiDesc</v>
       </c>
     </row>
     <row r="91" spans="8:30" x14ac:dyDescent="0.25">
       <c r="I91" s="1" t="str">
-        <f t="shared" ref="I91" si="30">IF(H63="+",I63,IF(H63="-","",IF(I63="","","??????")))</f>
+        <f t="shared" ref="I91" si="41">IF(H63="+",I63,IF(H63="-","",IF(I63="","","??????")))</f>
         <v/>
       </c>
       <c r="L91" s="1" t="str">
-        <f>IF(K63="+",L63,IF(K63="-","",IF(L63="","","??????")))</f>
+        <f t="shared" ref="L91:L116" si="42">IF(K63="+",L63,IF(K63="-","",IF(L63="","","??????")))</f>
         <v>AddonType</v>
       </c>
       <c r="O91" s="1" t="str">
@@ -3505,887 +3541,887 @@
         <v>AddonType</v>
       </c>
       <c r="R91" s="1" t="str">
-        <f t="shared" ref="R91:AD106" si="31">IF(Q63="+",R63,IF(Q63="-","",IF(R63="","","??????")))</f>
+        <f t="shared" ref="R91:AD106" si="43">IF(Q63="+",R63,IF(Q63="-","",IF(R63="","","??????")))</f>
         <v/>
       </c>
       <c r="U91" s="1" t="str">
-        <f t="shared" ref="U91" si="32">IF(T63="+",U63,IF(T63="-","",IF(U63="","","??????")))</f>
+        <f t="shared" ref="U91" si="44">IF(T63="+",U63,IF(T63="-","",IF(U63="","","??????")))</f>
         <v>UiDesc</v>
       </c>
       <c r="X91" s="1" t="str">
-        <f t="shared" ref="X91" si="33">IF(W63="+",X63,IF(W63="-","",IF(X63="","","??????")))</f>
+        <f t="shared" ref="X91" si="45">IF(W63="+",X63,IF(W63="-","",IF(X63="","","??????")))</f>
         <v/>
       </c>
       <c r="AA91" s="1" t="str">
-        <f t="shared" ref="AA91" si="34">IF(Z63="+",AA63,IF(Z63="-","",IF(AA63="","","??????")))</f>
+        <f t="shared" ref="AA91" si="46">IF(Z63="+",AA63,IF(Z63="-","",IF(AA63="","","??????")))</f>
         <v/>
       </c>
       <c r="AD91" s="1" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
     </row>
     <row r="92" spans="8:30" x14ac:dyDescent="0.25">
       <c r="I92" s="1" t="str">
-        <f t="shared" ref="I92:I106" si="35">IF(H64="+",I64,IF(H64="-","",IF(I64="","","??????")))</f>
+        <f t="shared" ref="I92:I106" si="47">IF(H64="+",I64,IF(H64="-","",IF(I64="","","??????")))</f>
         <v/>
       </c>
       <c r="L92" s="1" t="str">
-        <f>IF(K64="+",L64,IF(K64="-","",IF(L64="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O92" s="1" t="str">
-        <f t="shared" ref="O92:O99" si="36">IF(N64="+",O64,IF(N64="-","",IF(O64="","","??????")))</f>
+        <f t="shared" ref="O92:O99" si="48">IF(N64="+",O64,IF(N64="-","",IF(O64="","","??????")))</f>
         <v/>
       </c>
       <c r="R92" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="U92" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="X92" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AA92" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AD92" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
     <row r="93" spans="8:30" x14ac:dyDescent="0.25">
       <c r="I93" s="1" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v/>
       </c>
       <c r="L93" s="1" t="str">
-        <f>IF(K65="+",L65,IF(K65="-","",IF(L65="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v>InstallSocket</v>
       </c>
       <c r="O93" s="1" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="R93" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="U93" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="X93" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AA93" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AD93" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
     <row r="94" spans="8:30" x14ac:dyDescent="0.25">
       <c r="I94" s="1" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v>UiDesc</v>
       </c>
       <c r="L94" s="1" t="str">
-        <f>IF(K66="+",L66,IF(K66="-","",IF(L66="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v>LoadArea</v>
       </c>
       <c r="O94" s="1" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="48"/>
         <v>InstallSlot</v>
       </c>
       <c r="R94" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="U94" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="X94" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AA94" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AD94" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
     <row r="95" spans="8:30" x14ac:dyDescent="0.25">
       <c r="I95" s="1" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v/>
       </c>
       <c r="L95" s="1" t="str">
-        <f>IF(K67="+",L67,IF(K67="-","",IF(L67="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v>RequiredAddon</v>
       </c>
       <c r="O95" s="1" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="48"/>
         <v>InstallSocket</v>
       </c>
       <c r="R95" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="U95" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="X95" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AA95" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AD95" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
     <row r="96" spans="8:30" x14ac:dyDescent="0.25">
       <c r="I96" s="1" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v/>
       </c>
       <c r="L96" s="1" t="str">
-        <f>IF(K68="+",L68,IF(K68="-","",IF(L68="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O96" s="1" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="48"/>
         <v>LoadArea</v>
       </c>
       <c r="R96" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="U96" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="X96" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AA96" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AD96" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
     <row r="97" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I97" s="1" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v/>
       </c>
       <c r="L97" s="1" t="str">
-        <f>IF(K69="+",L69,IF(K69="-","",IF(L69="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O97" s="1" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="48"/>
         <v>RequiredAddon</v>
       </c>
       <c r="R97" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="U97" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="X97" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AA97" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AD97" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
     <row r="98" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I98" s="1" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v/>
       </c>
       <c r="L98" s="1" t="str">
-        <f>IF(K70="+",L70,IF(K70="-","",IF(L70="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O98" s="1" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="48"/>
         <v>RequiredAddonType</v>
       </c>
       <c r="R98" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="U98" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="X98" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AA98" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AD98" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
     <row r="99" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I99" s="1" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v/>
       </c>
       <c r="L99" s="1" t="str">
-        <f>IF(K71="+",L71,IF(K71="-","",IF(L71="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v>UiDesc</v>
       </c>
       <c r="O99" s="1" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="R99" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="U99" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="X99" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AA99" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AD99" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
     <row r="100" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I100" s="1" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v/>
       </c>
       <c r="L100" s="1" t="str">
-        <f>IF(K72="+",L72,IF(K72="-","",IF(L72="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O100" s="1" t="str">
-        <f t="shared" ref="O100" si="37">IF(N72="+",O72,IF(N72="-","",IF(O72="","","??????")))</f>
+        <f t="shared" ref="O100" si="49">IF(N72="+",O72,IF(N72="-","",IF(O72="","","??????")))</f>
         <v/>
       </c>
       <c r="R100" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="U100" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="X100" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AA100" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AD100" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
     <row r="101" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I101" s="1" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v/>
       </c>
       <c r="L101" s="1" t="str">
-        <f>IF(K73="+",L73,IF(K73="-","",IF(L73="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O101" s="1" t="str">
-        <f t="shared" ref="O101" si="38">IF(N73="+",O73,IF(N73="-","",IF(O73="","","??????")))</f>
+        <f t="shared" ref="O101" si="50">IF(N73="+",O73,IF(N73="-","",IF(O73="","","??????")))</f>
         <v/>
       </c>
       <c r="R101" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="U101" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="X101" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AA101" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AD101" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
     <row r="102" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I102" s="1" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v/>
       </c>
       <c r="L102" s="1" t="str">
-        <f>IF(K74="+",L74,IF(K74="-","",IF(L74="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O102" s="1" t="str">
-        <f t="shared" ref="O102" si="39">IF(N74="+",O74,IF(N74="-","",IF(O74="","","??????")))</f>
+        <f t="shared" ref="O102" si="51">IF(N74="+",O74,IF(N74="-","",IF(O74="","","??????")))</f>
         <v/>
       </c>
       <c r="R102" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="U102" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="X102" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AA102" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AD102" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
     <row r="103" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I103" s="1" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v/>
       </c>
       <c r="L103" s="1" t="str">
-        <f>IF(K75="+",L75,IF(K75="-","",IF(L75="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O103" s="1" t="str">
-        <f t="shared" ref="O103" si="40">IF(N75="+",O75,IF(N75="-","",IF(O75="","","??????")))</f>
+        <f t="shared" ref="O103" si="52">IF(N75="+",O75,IF(N75="-","",IF(O75="","","??????")))</f>
         <v/>
       </c>
       <c r="R103" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="U103" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="X103" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AA103" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AD103" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
     <row r="104" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I104" s="1" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v/>
       </c>
       <c r="L104" s="1" t="str">
-        <f>IF(K76="+",L76,IF(K76="-","",IF(L76="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O104" s="1" t="str">
-        <f t="shared" ref="O104" si="41">IF(N76="+",O76,IF(N76="-","",IF(O76="","","??????")))</f>
+        <f t="shared" ref="O104" si="53">IF(N76="+",O76,IF(N76="-","",IF(O76="","","??????")))</f>
         <v/>
       </c>
       <c r="R104" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="U104" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="X104" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AA104" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AD104" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
     <row r="105" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I105" s="1" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v/>
       </c>
       <c r="L105" s="1" t="str">
-        <f>IF(K77="+",L77,IF(K77="-","",IF(L77="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O105" s="1" t="str">
-        <f t="shared" ref="O105" si="42">IF(N77="+",O77,IF(N77="-","",IF(O77="","","??????")))</f>
+        <f t="shared" ref="O105" si="54">IF(N77="+",O77,IF(N77="-","",IF(O77="","","??????")))</f>
         <v/>
       </c>
       <c r="R105" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="U105" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="X105" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AA105" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AD105" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
     <row r="106" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I106" s="1" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="47"/>
         <v/>
       </c>
       <c r="L106" s="1" t="str">
-        <f>IF(K78="+",L78,IF(K78="-","",IF(L78="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O106" s="1" t="str">
-        <f t="shared" ref="O106" si="43">IF(N78="+",O78,IF(N78="-","",IF(O78="","","??????")))</f>
+        <f t="shared" ref="O106" si="55">IF(N78="+",O78,IF(N78="-","",IF(O78="","","??????")))</f>
         <v/>
       </c>
       <c r="R106" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="U106" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="X106" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AA106" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AD106" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
     <row r="107" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I107" s="1" t="str">
-        <f t="shared" ref="I107:I116" si="44">IF(H79="+",I79,IF(H79="-","",IF(I79="","","??????")))</f>
+        <f t="shared" ref="I107:I116" si="56">IF(H79="+",I79,IF(H79="-","",IF(I79="","","??????")))</f>
         <v/>
       </c>
       <c r="L107" s="1" t="str">
-        <f>IF(K79="+",L79,IF(K79="-","",IF(L79="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O107" s="1" t="str">
-        <f t="shared" ref="O107" si="45">IF(N79="+",O79,IF(N79="-","",IF(O79="","","??????")))</f>
+        <f t="shared" ref="O107" si="57">IF(N79="+",O79,IF(N79="-","",IF(O79="","","??????")))</f>
         <v/>
       </c>
       <c r="R107" s="1" t="str">
-        <f t="shared" ref="R107:AD116" si="46">IF(Q79="+",R79,IF(Q79="-","",IF(R79="","","??????")))</f>
+        <f t="shared" ref="R107:AD116" si="58">IF(Q79="+",R79,IF(Q79="-","",IF(R79="","","??????")))</f>
         <v/>
       </c>
       <c r="U107" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="X107" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AA107" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AD107" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
     </row>
     <row r="108" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I108" s="1" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="56"/>
         <v/>
       </c>
       <c r="L108" s="1" t="str">
-        <f>IF(K80="+",L80,IF(K80="-","",IF(L80="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O108" s="1" t="str">
-        <f t="shared" ref="O108" si="47">IF(N80="+",O80,IF(N80="-","",IF(O80="","","??????")))</f>
+        <f t="shared" ref="O108" si="59">IF(N80="+",O80,IF(N80="-","",IF(O80="","","??????")))</f>
         <v/>
       </c>
       <c r="R108" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="U108" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="X108" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AA108" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AD108" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
     </row>
     <row r="109" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I109" s="1" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="56"/>
         <v/>
       </c>
       <c r="L109" s="1" t="str">
-        <f>IF(K81="+",L81,IF(K81="-","",IF(L81="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O109" s="1" t="str">
-        <f t="shared" ref="O109" si="48">IF(N81="+",O81,IF(N81="-","",IF(O81="","","??????")))</f>
+        <f t="shared" ref="O109" si="60">IF(N81="+",O81,IF(N81="-","",IF(O81="","","??????")))</f>
         <v/>
       </c>
       <c r="R109" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="U109" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="X109" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AA109" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AD109" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
     </row>
     <row r="110" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I110" s="1" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="56"/>
         <v/>
       </c>
       <c r="L110" s="1" t="str">
-        <f>IF(K82="+",L82,IF(K82="-","",IF(L82="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O110" s="1" t="str">
-        <f t="shared" ref="O110" si="49">IF(N82="+",O82,IF(N82="-","",IF(O82="","","??????")))</f>
+        <f t="shared" ref="O110" si="61">IF(N82="+",O82,IF(N82="-","",IF(O82="","","??????")))</f>
         <v/>
       </c>
       <c r="R110" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="U110" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="X110" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AA110" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AD110" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
     </row>
     <row r="111" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I111" s="1" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="56"/>
         <v/>
       </c>
       <c r="L111" s="1" t="str">
-        <f>IF(K83="+",L83,IF(K83="-","",IF(L83="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O111" s="1" t="str">
-        <f t="shared" ref="O111" si="50">IF(N83="+",O83,IF(N83="-","",IF(O83="","","??????")))</f>
+        <f t="shared" ref="O111" si="62">IF(N83="+",O83,IF(N83="-","",IF(O83="","","??????")))</f>
         <v/>
       </c>
       <c r="R111" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="U111" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="X111" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AA111" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AD111" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
     </row>
     <row r="112" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I112" s="1" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="56"/>
         <v/>
       </c>
       <c r="L112" s="1" t="str">
-        <f>IF(K84="+",L84,IF(K84="-","",IF(L84="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O112" s="1" t="str">
-        <f t="shared" ref="O112" si="51">IF(N84="+",O84,IF(N84="-","",IF(O84="","","??????")))</f>
+        <f t="shared" ref="O112" si="63">IF(N84="+",O84,IF(N84="-","",IF(O84="","","??????")))</f>
         <v/>
       </c>
       <c r="R112" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="U112" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="X112" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AA112" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AD112" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
     </row>
     <row r="113" spans="2:30" x14ac:dyDescent="0.25">
       <c r="I113" s="1" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="56"/>
         <v/>
       </c>
       <c r="L113" s="1" t="str">
-        <f>IF(K85="+",L85,IF(K85="-","",IF(L85="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O113" s="1" t="str">
-        <f t="shared" ref="O113" si="52">IF(N85="+",O85,IF(N85="-","",IF(O85="","","??????")))</f>
+        <f t="shared" ref="O113" si="64">IF(N85="+",O85,IF(N85="-","",IF(O85="","","??????")))</f>
         <v/>
       </c>
       <c r="R113" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="U113" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="X113" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AA113" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AD113" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
     </row>
     <row r="114" spans="2:30" x14ac:dyDescent="0.25">
       <c r="I114" s="1" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="56"/>
         <v/>
       </c>
       <c r="L114" s="1" t="str">
-        <f>IF(K86="+",L86,IF(K86="-","",IF(L86="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O114" s="1" t="str">
-        <f t="shared" ref="O114" si="53">IF(N86="+",O86,IF(N86="-","",IF(O86="","","??????")))</f>
+        <f t="shared" ref="O114" si="65">IF(N86="+",O86,IF(N86="-","",IF(O86="","","??????")))</f>
         <v>SpawnLoadOrigin</v>
       </c>
       <c r="R114" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="U114" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="X114" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AA114" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AD114" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
     </row>
     <row r="115" spans="2:30" x14ac:dyDescent="0.25">
       <c r="I115" s="1" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="56"/>
         <v/>
       </c>
       <c r="L115" s="1" t="str">
-        <f>IF(K87="+",L87,IF(K87="-","",IF(L87="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O115" s="1" t="str">
-        <f t="shared" ref="O115" si="54">IF(N87="+",O87,IF(N87="-","",IF(O87="","","??????")))</f>
+        <f t="shared" ref="O115" si="66">IF(N87="+",O87,IF(N87="-","",IF(O87="","","??????")))</f>
         <v>UiDesc</v>
       </c>
       <c r="R115" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="U115" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="X115" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AA115" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AD115" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
     </row>
     <row r="116" spans="2:30" x14ac:dyDescent="0.25">
       <c r="I116" s="1" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="56"/>
         <v/>
       </c>
       <c r="L116" s="1" t="str">
-        <f>IF(K88="+",L88,IF(K88="-","",IF(L88="","","??????")))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="O116" s="1" t="str">
-        <f t="shared" ref="O116" si="55">IF(N88="+",O88,IF(N88="-","",IF(O88="","","??????")))</f>
+        <f t="shared" ref="O116" si="67">IF(N88="+",O88,IF(N88="-","",IF(O88="","","??????")))</f>
         <v/>
       </c>
       <c r="R116" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="U116" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="X116" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AA116" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="AD116" s="1" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
     </row>
     <row r="118" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B118">
-        <f>SUMIF(I118:AD118,$E118,I$1:AD$1)</f>
+        <f t="shared" ref="B118:B126" si="68">SUMIF(I118:AD118,$E118,I$1:AD$1)</f>
         <v>8</v>
       </c>
       <c r="C118">
-        <f>SUMIF(I118:AD118,$E118,I$2:AD$2)</f>
+        <f t="shared" ref="C118:C126" si="69">SUMIF(I118:AD118,$E118,I$2:AD$2)</f>
         <v>255</v>
       </c>
       <c r="D118" s="4" t="str">
-        <f>TEXT(B118,"00")&amp;"_"&amp;TEXT(C118,"0000")</f>
+        <f t="shared" ref="D118:D126" si="70">TEXT(B118,"00")&amp;"_"&amp;TEXT(C118,"0000")</f>
         <v>08_0255</v>
       </c>
       <c r="E118" t="s">
@@ -4395,49 +4431,49 @@
         <v>66</v>
       </c>
       <c r="I118" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E118,I$62:I$88,0)),"",$E118)</f>
+        <f t="shared" ref="I118:I126" si="71">IF(ISERROR(MATCH($E118,I$62:I$88,0)),"",$E118)</f>
         <v>UiDesc</v>
       </c>
       <c r="L118" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E118,L$62:L$88,0)),"",$E118)</f>
+        <f t="shared" ref="L118:L126" si="72">IF(ISERROR(MATCH($E118,L$62:L$88,0)),"",$E118)</f>
         <v>UiDesc</v>
       </c>
       <c r="O118" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E118,O$62:O$88,0)),"",$E118)</f>
+        <f t="shared" ref="O118:O126" si="73">IF(ISERROR(MATCH($E118,O$62:O$88,0)),"",$E118)</f>
         <v>UiDesc</v>
       </c>
       <c r="R118" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E118,R$62:R$88,0)),"",$E118)</f>
+        <f t="shared" ref="R118:R126" si="74">IF(ISERROR(MATCH($E118,R$62:R$88,0)),"",$E118)</f>
         <v>UiDesc</v>
       </c>
       <c r="U118" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E118,U$62:U$88,0)),"",$E118)</f>
+        <f t="shared" ref="U118:U126" si="75">IF(ISERROR(MATCH($E118,U$62:U$88,0)),"",$E118)</f>
         <v>UiDesc</v>
       </c>
       <c r="X118" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E118,X$62:X$88,0)),"",$E118)</f>
+        <f t="shared" ref="X118:X126" si="76">IF(ISERROR(MATCH($E118,X$62:X$88,0)),"",$E118)</f>
         <v>UiDesc</v>
       </c>
       <c r="AA118" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E118,AA$62:AA$88,0)),"",$E118)</f>
+        <f t="shared" ref="AA118:AA126" si="77">IF(ISERROR(MATCH($E118,AA$62:AA$88,0)),"",$E118)</f>
         <v>UiDesc</v>
       </c>
       <c r="AD118" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E118,AD$62:AD$88,0)),"",$E118)</f>
+        <f t="shared" ref="AD118:AD126" si="78">IF(ISERROR(MATCH($E118,AD$62:AD$88,0)),"",$E118)</f>
         <v>UiDesc</v>
       </c>
     </row>
     <row r="119" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B119">
-        <f>SUMIF(I119:AD119,$E119,I$1:AD$1)</f>
+        <f t="shared" si="68"/>
         <v>3</v>
       </c>
       <c r="C119">
-        <f>SUMIF(I119:AD119,$E119,I$2:AD$2)</f>
+        <f t="shared" si="69"/>
         <v>7</v>
       </c>
       <c r="D119" s="4" t="str">
-        <f>TEXT(B119,"00")&amp;"_"&amp;TEXT(C119,"0000")</f>
+        <f t="shared" si="70"/>
         <v>03_0007</v>
       </c>
       <c r="E119" t="s">
@@ -4447,49 +4483,49 @@
         <v>67</v>
       </c>
       <c r="I119" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E119,I$62:I$88,0)),"",$E119)</f>
+        <f t="shared" si="71"/>
         <v>AddonSlots</v>
       </c>
       <c r="L119" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E119,L$62:L$88,0)),"",$E119)</f>
+        <f t="shared" si="72"/>
         <v>AddonSlots</v>
       </c>
       <c r="O119" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E119,O$62:O$88,0)),"",$E119)</f>
+        <f t="shared" si="73"/>
         <v>AddonSlots</v>
       </c>
       <c r="R119" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E119,R$62:R$88,0)),"",$E119)</f>
+        <f t="shared" si="74"/>
         <v/>
       </c>
       <c r="U119" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E119,U$62:U$88,0)),"",$E119)</f>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="X119" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E119,X$62:X$88,0)),"",$E119)</f>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="AA119" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E119,AA$62:AA$88,0)),"",$E119)</f>
+        <f t="shared" si="77"/>
         <v/>
       </c>
       <c r="AD119" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E119,AD$62:AD$88,0)),"",$E119)</f>
+        <f t="shared" si="78"/>
         <v/>
       </c>
     </row>
     <row r="120" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B120">
-        <f>SUMIF(I120:AD120,$E120,I$1:AD$1)</f>
+        <f t="shared" si="68"/>
         <v>2</v>
       </c>
       <c r="C120">
-        <f>SUMIF(I120:AD120,$E120,I$2:AD$2)</f>
+        <f t="shared" si="69"/>
         <v>6</v>
       </c>
       <c r="D120" s="4" t="str">
-        <f>TEXT(B120,"00")&amp;"_"&amp;TEXT(C120,"0000")</f>
+        <f t="shared" si="70"/>
         <v>02_0006</v>
       </c>
       <c r="E120" t="s">
@@ -4499,49 +4535,49 @@
         <v>68</v>
       </c>
       <c r="I120" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E120,I$62:I$88,0)),"",$E120)</f>
+        <f t="shared" si="71"/>
         <v/>
       </c>
       <c r="L120" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E120,L$62:L$88,0)),"",$E120)</f>
+        <f t="shared" si="72"/>
         <v>AddonType</v>
       </c>
       <c r="O120" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E120,O$62:O$88,0)),"",$E120)</f>
+        <f t="shared" si="73"/>
         <v>AddonType</v>
       </c>
       <c r="R120" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E120,R$62:R$88,0)),"",$E120)</f>
+        <f t="shared" si="74"/>
         <v/>
       </c>
       <c r="U120" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E120,U$62:U$88,0)),"",$E120)</f>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="X120" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E120,X$62:X$88,0)),"",$E120)</f>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="AA120" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E120,AA$62:AA$88,0)),"",$E120)</f>
+        <f t="shared" si="77"/>
         <v/>
       </c>
       <c r="AD120" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E120,AD$62:AD$88,0)),"",$E120)</f>
+        <f t="shared" si="78"/>
         <v/>
       </c>
     </row>
     <row r="121" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B121">
-        <f>SUMIF(I121:AD121,$E121,I$1:AD$1)</f>
+        <f t="shared" si="68"/>
         <v>2</v>
       </c>
       <c r="C121">
-        <f>SUMIF(I121:AD121,$E121,I$2:AD$2)</f>
+        <f t="shared" si="69"/>
         <v>6</v>
       </c>
       <c r="D121" s="4" t="str">
-        <f>TEXT(B121,"00")&amp;"_"&amp;TEXT(C121,"0000")</f>
+        <f t="shared" si="70"/>
         <v>02_0006</v>
       </c>
       <c r="E121" t="s">
@@ -4551,49 +4587,49 @@
         <v>68</v>
       </c>
       <c r="I121" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E121,I$62:I$88,0)),"",$E121)</f>
+        <f t="shared" si="71"/>
         <v/>
       </c>
       <c r="L121" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E121,L$62:L$88,0)),"",$E121)</f>
+        <f t="shared" si="72"/>
         <v>InstallSocket</v>
       </c>
       <c r="O121" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E121,O$62:O$88,0)),"",$E121)</f>
+        <f t="shared" si="73"/>
         <v>InstallSocket</v>
       </c>
       <c r="R121" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E121,R$62:R$88,0)),"",$E121)</f>
+        <f t="shared" si="74"/>
         <v/>
       </c>
       <c r="U121" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E121,U$62:U$88,0)),"",$E121)</f>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="X121" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E121,X$62:X$88,0)),"",$E121)</f>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="AA121" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E121,AA$62:AA$88,0)),"",$E121)</f>
+        <f t="shared" si="77"/>
         <v/>
       </c>
       <c r="AD121" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E121,AD$62:AD$88,0)),"",$E121)</f>
+        <f t="shared" si="78"/>
         <v/>
       </c>
     </row>
     <row r="122" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B122">
-        <f>SUMIF(I122:AD122,$E122,I$1:AD$1)</f>
+        <f t="shared" si="68"/>
         <v>2</v>
       </c>
       <c r="C122">
-        <f>SUMIF(I122:AD122,$E122,I$2:AD$2)</f>
+        <f t="shared" si="69"/>
         <v>6</v>
       </c>
       <c r="D122" s="4" t="str">
-        <f>TEXT(B122,"00")&amp;"_"&amp;TEXT(C122,"0000")</f>
+        <f t="shared" si="70"/>
         <v>02_0006</v>
       </c>
       <c r="E122" t="s">
@@ -4603,49 +4639,49 @@
         <v>68</v>
       </c>
       <c r="I122" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E122,I$62:I$88,0)),"",$E122)</f>
+        <f t="shared" si="71"/>
         <v/>
       </c>
       <c r="L122" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E122,L$62:L$88,0)),"",$E122)</f>
+        <f t="shared" si="72"/>
         <v>LoadArea</v>
       </c>
       <c r="O122" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E122,O$62:O$88,0)),"",$E122)</f>
+        <f t="shared" si="73"/>
         <v>LoadArea</v>
       </c>
       <c r="R122" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E122,R$62:R$88,0)),"",$E122)</f>
+        <f t="shared" si="74"/>
         <v/>
       </c>
       <c r="U122" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E122,U$62:U$88,0)),"",$E122)</f>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="X122" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E122,X$62:X$88,0)),"",$E122)</f>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="AA122" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E122,AA$62:AA$88,0)),"",$E122)</f>
+        <f t="shared" si="77"/>
         <v/>
       </c>
       <c r="AD122" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E122,AD$62:AD$88,0)),"",$E122)</f>
+        <f t="shared" si="78"/>
         <v/>
       </c>
     </row>
     <row r="123" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B123">
-        <f>SUMIF(I123:AD123,$E123,I$1:AD$1)</f>
+        <f t="shared" si="68"/>
         <v>2</v>
       </c>
       <c r="C123">
-        <f>SUMIF(I123:AD123,$E123,I$2:AD$2)</f>
+        <f t="shared" si="69"/>
         <v>6</v>
       </c>
       <c r="D123" s="4" t="str">
-        <f>TEXT(B123,"00")&amp;"_"&amp;TEXT(C123,"0000")</f>
+        <f t="shared" si="70"/>
         <v>02_0006</v>
       </c>
       <c r="E123" t="s">
@@ -4655,182 +4691,191 @@
         <v>68</v>
       </c>
       <c r="I123" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E123,I$62:I$88,0)),"",$E123)</f>
+        <f t="shared" si="71"/>
         <v/>
       </c>
       <c r="L123" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E123,L$62:L$88,0)),"",$E123)</f>
+        <f t="shared" si="72"/>
         <v>RequiredAddon</v>
       </c>
       <c r="O123" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E123,O$62:O$88,0)),"",$E123)</f>
+        <f t="shared" si="73"/>
         <v>RequiredAddon</v>
       </c>
       <c r="R123" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E123,R$62:R$88,0)),"",$E123)</f>
+        <f t="shared" si="74"/>
         <v/>
       </c>
       <c r="U123" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E123,U$62:U$88,0)),"",$E123)</f>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="X123" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E123,X$62:X$88,0)),"",$E123)</f>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="AA123" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E123,AA$62:AA$88,0)),"",$E123)</f>
+        <f t="shared" si="77"/>
         <v/>
       </c>
       <c r="AD123" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E123,AD$62:AD$88,0)),"",$E123)</f>
+        <f t="shared" si="78"/>
         <v/>
       </c>
     </row>
     <row r="124" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B124">
-        <f>SUMIF(I124:AD124,$E124,I$1:AD$1)</f>
+        <f t="shared" si="68"/>
         <v>1</v>
       </c>
       <c r="C124">
-        <f>SUMIF(I124:AD124,$E124,I$2:AD$2)</f>
+        <f t="shared" si="69"/>
         <v>4</v>
       </c>
       <c r="D124" s="4" t="str">
-        <f>TEXT(B124,"00")&amp;"_"&amp;TEXT(C124,"0000")</f>
+        <f t="shared" si="70"/>
         <v>01_0004</v>
       </c>
       <c r="E124" t="s">
         <v>41</v>
       </c>
+      <c r="F124" t="s">
+        <v>71</v>
+      </c>
       <c r="I124" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E124,I$62:I$88,0)),"",$E124)</f>
+        <f t="shared" si="71"/>
         <v/>
       </c>
       <c r="L124" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E124,L$62:L$88,0)),"",$E124)</f>
+        <f t="shared" si="72"/>
         <v/>
       </c>
       <c r="O124" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E124,O$62:O$88,0)),"",$E124)</f>
+        <f t="shared" si="73"/>
         <v>InstallSlot</v>
       </c>
       <c r="R124" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E124,R$62:R$88,0)),"",$E124)</f>
+        <f t="shared" si="74"/>
         <v/>
       </c>
       <c r="U124" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E124,U$62:U$88,0)),"",$E124)</f>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="X124" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E124,X$62:X$88,0)),"",$E124)</f>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="AA124" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E124,AA$62:AA$88,0)),"",$E124)</f>
+        <f t="shared" si="77"/>
         <v/>
       </c>
       <c r="AD124" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E124,AD$62:AD$88,0)),"",$E124)</f>
+        <f t="shared" si="78"/>
         <v/>
       </c>
     </row>
     <row r="125" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B125">
-        <f>SUMIF(I125:AD125,$E125,I$1:AD$1)</f>
+        <f t="shared" si="68"/>
         <v>1</v>
       </c>
       <c r="C125">
-        <f>SUMIF(I125:AD125,$E125,I$2:AD$2)</f>
+        <f t="shared" si="69"/>
         <v>4</v>
       </c>
       <c r="D125" s="4" t="str">
-        <f>TEXT(B125,"00")&amp;"_"&amp;TEXT(C125,"0000")</f>
+        <f t="shared" si="70"/>
         <v>01_0004</v>
       </c>
       <c r="E125" t="s">
         <v>42</v>
       </c>
+      <c r="F125" t="s">
+        <v>71</v>
+      </c>
       <c r="I125" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E125,I$62:I$88,0)),"",$E125)</f>
+        <f t="shared" si="71"/>
         <v/>
       </c>
       <c r="L125" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E125,L$62:L$88,0)),"",$E125)</f>
+        <f t="shared" si="72"/>
         <v/>
       </c>
       <c r="O125" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E125,O$62:O$88,0)),"",$E125)</f>
+        <f t="shared" si="73"/>
         <v>RequiredAddonType</v>
       </c>
       <c r="R125" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E125,R$62:R$88,0)),"",$E125)</f>
+        <f t="shared" si="74"/>
         <v/>
       </c>
       <c r="U125" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E125,U$62:U$88,0)),"",$E125)</f>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="X125" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E125,X$62:X$88,0)),"",$E125)</f>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="AA125" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E125,AA$62:AA$88,0)),"",$E125)</f>
+        <f t="shared" si="77"/>
         <v/>
       </c>
       <c r="AD125" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E125,AD$62:AD$88,0)),"",$E125)</f>
+        <f t="shared" si="78"/>
         <v/>
       </c>
     </row>
     <row r="126" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B126">
-        <f>SUMIF(I126:AD126,$E126,I$1:AD$1)</f>
+        <f t="shared" si="68"/>
         <v>1</v>
       </c>
       <c r="C126">
-        <f>SUMIF(I126:AD126,$E126,I$2:AD$2)</f>
+        <f t="shared" si="69"/>
         <v>4</v>
       </c>
       <c r="D126" s="4" t="str">
-        <f>TEXT(B126,"00")&amp;"_"&amp;TEXT(C126,"0000")</f>
+        <f t="shared" si="70"/>
         <v>01_0004</v>
       </c>
       <c r="E126" t="s">
         <v>55</v>
       </c>
+      <c r="F126" t="s">
+        <v>71</v>
+      </c>
       <c r="I126" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E126,I$62:I$88,0)),"",$E126)</f>
+        <f t="shared" si="71"/>
         <v/>
       </c>
       <c r="L126" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E126,L$62:L$88,0)),"",$E126)</f>
+        <f t="shared" si="72"/>
         <v/>
       </c>
       <c r="O126" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E126,O$62:O$88,0)),"",$E126)</f>
+        <f t="shared" si="73"/>
         <v>SpawnLoadOrigin</v>
       </c>
       <c r="R126" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E126,R$62:R$88,0)),"",$E126)</f>
+        <f t="shared" si="74"/>
         <v/>
       </c>
       <c r="U126" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E126,U$62:U$88,0)),"",$E126)</f>
+        <f t="shared" si="75"/>
         <v/>
       </c>
       <c r="X126" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E126,X$62:X$88,0)),"",$E126)</f>
+        <f t="shared" si="76"/>
         <v/>
       </c>
       <c r="AA126" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E126,AA$62:AA$88,0)),"",$E126)</f>
+        <f t="shared" si="77"/>
         <v/>
       </c>
       <c r="AD126" s="1" t="str">
-        <f>IF(ISERROR(MATCH($E126,AD$62:AD$88,0)),"",$E126)</f>
+        <f t="shared" si="78"/>
         <v/>
       </c>
     </row>

</xml_diff>